<commit_message>
add unl schedule info
</commit_message>
<xml_diff>
--- a/conferences/AP-LS_2024_Program.xlsx
+++ b/conferences/AP-LS_2024_Program.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/docs/apls-org/conferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA2A4D8-6737-D448-B837-59D9012B65BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44FFDBB-BD89-9B4F-AA17-4778DA2A32DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="760" windowWidth="30440" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4120" yWindow="760" windowWidth="30440" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2062" uniqueCount="943">
   <si>
     <t>date</t>
   </si>
@@ -2867,6 +2867,9 @@
   </si>
   <si>
     <t>Break</t>
+  </si>
+  <si>
+    <t>Celebrating 50 years! (1974-2024)</t>
   </si>
 </sst>
 </file>
@@ -3350,8 +3353,8 @@
   </sheetPr>
   <dimension ref="A1:X155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G39" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" topLeftCell="E87" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7935,7 +7938,9 @@
       <c r="I94" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J94" s="2"/>
+      <c r="J94" s="2" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="95" spans="1:24" ht="13">
       <c r="A95" s="3">

</xml_diff>

<commit_message>
fix table, add jobs
</commit_message>
<xml_diff>
--- a/conferences/AP-LS_2024_Program.xlsx
+++ b/conferences/AP-LS_2024_Program.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/docs/apls-org/conferences/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44FFDBB-BD89-9B4F-AA17-4778DA2A32DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A16D4B0-F883-F14F-B605-C4A54114E91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="760" windowWidth="30440" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11740" yWindow="3040" windowWidth="38760" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -3353,8 +3353,8 @@
   </sheetPr>
   <dimension ref="A1:X155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E87" zoomScale="117" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>